<commit_message>
stu converted bib months to bibtex months, recompile (no errors)
month info:
ftp://ftp.tex.ac.uk/tex-archive/biblio/bibtex/contrib/doc/btxFAQ.pdf
</commit_message>
<xml_diff>
--- a/BriefTasks 2013-07-30.xlsx
+++ b/BriefTasks 2013-07-30.xlsx
@@ -576,8 +576,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="171">
+  <cellStyleXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -851,7 +853,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="171">
+  <cellStyles count="173">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -937,6 +939,7 @@
     <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1022,6 +1025,7 @@
     <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1353,8 +1357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="H99" sqref="H99"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:XFD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2205,18 +2209,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="2" t="s">
+    <row r="44" spans="1:7" hidden="1">
+      <c r="A44" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="B44" s="22" t="s">
+      <c r="B44" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="G44" s="1" t="s">
-        <v>17</v>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:7" hidden="1">
@@ -2477,37 +2484,45 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
-      <c r="A58" s="2">
+    <row r="58" spans="1:7" hidden="1">
+      <c r="A58" s="13">
         <v>5</v>
       </c>
-      <c r="B58" s="22" t="s">
+      <c r="B58" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="D58" s="3">
+      <c r="D58" s="15">
         <v>41449</v>
       </c>
-      <c r="G58" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
-      <c r="A59" s="2">
+      <c r="E58" s="15">
+        <v>41496</v>
+      </c>
+      <c r="F58" s="16"/>
+      <c r="G58" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" hidden="1">
+      <c r="A59" s="13">
         <v>5</v>
       </c>
-      <c r="B59" s="22" t="s">
+      <c r="B59" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="D59" s="3">
+      <c r="D59" s="15">
         <v>41449</v>
       </c>
-      <c r="G59" s="1" t="s">
+      <c r="E59" s="15">
+        <v>41496</v>
+      </c>
+      <c r="F59" s="16"/>
+      <c r="G59" s="14" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>